<commit_message>
Fix typo in word cloud
</commit_message>
<xml_diff>
--- a/word_cloud_weights.xlsx
+++ b/word_cloud_weights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohan/mohanliu.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90A05B7-7225-3543-AE65-6D4486CEA1CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58C6181-9380-1F40-AF45-C943640247D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{67E4BAEB-0AA2-5B44-B189-53558797203D}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>sckit-learn</t>
-  </si>
-  <si>
     <t>C++</t>
   </si>
   <si>
@@ -93,18 +90,12 @@
     <t>SVM</t>
   </si>
   <si>
-    <t>Gradient Boost</t>
-  </si>
-  <si>
     <t>PCA</t>
   </si>
   <si>
     <t>XGBOOST</t>
   </si>
   <si>
-    <t>LightBGM</t>
-  </si>
-  <si>
     <t>NLTK</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>MongoDB</t>
   </si>
   <si>
-    <t>Web design</t>
-  </si>
-  <si>
     <t>GUI</t>
   </si>
   <si>
@@ -135,7 +123,19 @@
     <t>Keras</t>
   </si>
   <si>
-    <t>Web scrapping</t>
+    <t>scikit-learn</t>
+  </si>
+  <si>
+    <t>Web Design</t>
+  </si>
+  <si>
+    <t>Web Scrapping</t>
+  </si>
+  <si>
+    <t>LightGBM</t>
+  </si>
+  <si>
+    <t>GBDT</t>
   </si>
 </sst>
 </file>
@@ -490,12 +490,12 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B35" sqref="A4:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>80</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>85</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>83</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>82</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>60</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>60</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>68</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>90</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>80</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>60</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>40</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>42</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>78</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>70</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>82</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>68</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>75</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>77</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>40</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <v>70</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25">
         <v>50</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>40</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>70</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>80</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29">
         <v>82</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>30</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31">
         <v>60</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B32">
         <v>40</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B33">
         <v>40</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B34">
         <v>50</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>70</v>

</xml_diff>